<commit_message>
feat(stress_des_deploy): auto deploy stress des table in docs
</commit_message>
<xml_diff>
--- a/checklists/stress_des.xlsx
+++ b/checklists/stress_des.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\HSMA\_Student_Code\jw_hsma_des_stroke_project\checklists\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F8588536-58DF-4B8C-972D-EFBC7B3C37DB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D5EDD754-391B-4394-AC79-81229EC4085C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="15720" xr2:uid="{5032E51A-F114-42AC-8875-B84ED91CA331}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="81">
   <si>
     <t> Strengthening the Reporting of Empirical Simulation Studies (STRESS)</t>
   </si>
@@ -51,9 +51,6 @@
   </si>
   <si>
     <t>Recommendation</t>
-  </si>
-  <si>
-    <t>Details (for us to fill in)</t>
   </si>
   <si>
     <r>
@@ -340,81 +337,6 @@
   </si>
   <si>
     <t>See diagram 2.1 in folder 'checklists' within GitHub repository</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">A single class of patient is used within the model, referenced as 'Patient' within the Python model code.
-These entities are the stroke and non-stroke patients who are seen within the pathway. 
-Key attributes are as follows:
-ID - a persistent identifier used to track a single patient through their full system journey
-q_time_nurse = Time spent waiting for nursing assessment or consultation.
-q_time_ward = Time spent waiting for an inpatient ward bed.
-onset_type = Categorisation of onset information: 0 : Known onset; 1 : Unknown onset but within CTP window; 2 : Unknown onset and outside CTP window
-mrs_type =  Modified Rankin Scale score at presentation (0–5). Drawn from an exponential distribution and capped at 5.  0 indicates no disability, while 5 represents severe disability. 
-mrs_discharge = Modified Rankin Scale score at discharge. Unlike mrs_type, which is set on patient generation, the mrs_discharge is set later by the model and may differ depending on the availability of different pathways within the model - e.g. a patient may have a lower MRS on discharge if the CT perfusion scanner availability permits them to have thrombolysis. 
-diagnosis = Raw randomised diagnostic value (0–100). 
-patient_diagnosis = Encoded diagnosis category: 0 : Intracerebral haemorrhage (ICH); 1 : Ischaemic stroke (I); 2 : Transient ischaemic attack (TIA); 3 : Stroke mimic; 4 : Non-stroke. This is mapped from the diagnosis patient attribute, using thresholds defined in the global parameter class `g`. 
-non_admission = a numerical score used to determine whether patients with a transient ischaemic attack (TIA) or stroke mimic symptoms are admitted. 
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Aptos"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">Tracking attributes
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Aptos"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">Various attributes are set as events occur in the model, allowing for post-hoc analysis of logs. 
-advanced_ct_pathway: Whether the patient enters an advanced CT imaging pathway (elsewhere referred to as CT perfusion scanning).
-sdec_pathway: Whether the patient is routed through the Same Day Emergency Care (SDEC) pathway.
-thrombolysis: Whether the patient receives thrombolysis.
-admission_avoidance: Whether the patient avoids an admission by being seen in SDEC instead.
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Aptos"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">Unused attributes
-</t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Aptos"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">Several attributes are created but not currently used by the published version of the model. They may be used in future versions of the model. </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Aptos"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">
-priority = a numerical triage priority level used for queue ordering. 
-thrombectomy = whether the patient receives mechanical thrombectomy
-</t>
-    </r>
   </si>
   <si>
     <r>
@@ -982,79 +904,217 @@
 If a bed is not available in the main stroke unit when required, patients will queue for a bed in the stroke unit, with the delay in being allocated a stroke bed being recorded as one of the key metrics in the model. Patients will wait indefinitely for a bed to become available. The duration of their stay in the main stroke unit is only sampled after a bed becomes available, and is independent of the time they spend waiting for a bed. [TODO: determine if this is the optimum behaviour]</t>
   </si>
   <si>
-    <r>
-      <t xml:space="preserve">Note that the time units used within the model are minutes; all values below relate to durations in minutes. </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="9"/>
-        <color theme="1"/>
-        <rFont val="Aptos"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">
-Patient inter-arrival times</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="9"/>
-        <color theme="1"/>
-        <rFont val="Aptos"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">
-Inter-arrival times are drawn from an exponential distribution. 
-Two different distributions are used for different times of day: 
-High arrival hours (7am to 11.59pm): λ = 1 / 200.0
-Low arrival hours (12am to 6.59am): λ = 1 / 666.666666666667
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="9"/>
-        <color theme="1"/>
-        <rFont val="Aptos"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">Activity durations </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="9"/>
-        <color theme="1"/>
-        <rFont val="Aptos"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">
-All activity durations draw from an exponential distribution, where λ is calculated as 1 divided by the relevant value from the list below. 
-mean_n_consult_time = 60
-mean_n_ct_time = 20
-mean_n_sdec_time = 240
-Time on the main wards is an exponential distribution parameterised in the same way, but the value depends on both the stroke type (intercranial haemhorragic [ich], ischaemic [i], transient ischaemic attack (tia), and stroke mimic or non-stroke. 
-mean_n_i_ward_time_mrs_0 = 1440 * 6
-mean_n_i_ward_time_mrs_1 = 1440 * 4
-mean_n_i_ward_time_mrs_2 = 1440 * 8
-mean_n_i_ward_time_mrs_3 = 1440 * 11
-mean_n_i_ward_time_mrs_4 = 1440 * 24
-mean_n_i_ward_time_mrs_5 = 1440 * 29
-mean_n_ich_ward_time_mrs_0 = 1440 * 5
-mean_n_ich_ward_time_mrs_1 = 1440 * 4
-mean_n_ich_ward_time_mrs_2 = 1440 * 5
-mean_n_ich_ward_time_mrs_3 = 1440 * 17
-mean_n_ich_ward_time_mrs_4 = 1440 * 36
-mean_n_ich_ward_time_mrs_5 = 1440 * 36
-mean_n_non_stroke_ward_time = 4320
-mean_n_tia_ward_time = 1440</t>
-    </r>
-  </si>
-  <si>
     <t xml:space="preserve">Nurse triage = generated entities undergo assessment by a nurse for a generated amount of time. Duration is generated using an exponential distribution parameterised from historical data. 
 CT or CT perfusion scanning = after triage, entities leave the nurse and undergo either a CT or CT perfusion (advanced CT) scan for a generated amount of time. Duration is generated using an exponential distribution parameterised from historical data. 
 Thrombolysis = if eligible, patients will undergo thrombolysis. The time taken for this is not modelled; it purely affects eventual LOS if patients are admitted to the stroke ward.
 Same Day Emergency Care (SDEC) = if SDEC is open and has capacity, all patients are admitted to the SDEC after scanning. 
 Ward stay = if admission is not avoided (see 2.5.3), entities are admitted to the main stroke ward for a generated amount of time. Patients may go straight from the CT/CTP scanning step if the SDEC is not open or is at capacity, or may move from the SDEC to the main ward. LOS is generated using an exponential distribution parameterised from historical data, stratified by Modified Rankin Scale on admission and stroke type, and adjusted by a defined proportion if thrombolysis is administered. </t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Note that the time units used within the model are minutes; all values below relate to durations in minutes.  An asterisk is used to identify those parameters that can be easily altered using the web based front end. All listed parameters could bechanged within the model code. </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="8"/>
+        <color theme="1"/>
+        <rFont val="Aptos"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">
+Patient inter-arrival times</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color theme="1"/>
+        <rFont val="Aptos"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">
+Inter-arrival times are drawn from an exponential distribution. 
+Two different distributions are used for different times of day: 
+* High arrival hours (7am to 11.59pm): λ = 1 / 200.0
+* Low arrival hours (12am to 6.59am): λ = 1 / 666.666666666667
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="8"/>
+        <color theme="1"/>
+        <rFont val="Aptos"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">Activity durations </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color theme="1"/>
+        <rFont val="Aptos"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">
+All activity durations draw from an exponential distribution, where λ is calculated as 1 divided by the relevant value from the list below (where all values relate to a number of minutes). 
+mean_n_consult_time = 60; mean_n_ct_time = 20; mean_n_sdec_time = 240
+Time on the main wards is an exponential distribution parameterised in the same way, but the value depends on both the stroke type (intercranial haemhorragic [ich], ischaemic [i], transient ischaemic attack (tia), and stroke mimic or non-stroke. 
+Ischaemic strokes: mrs_0 = 1440 * 6;  mrs_1 = 1440 * 4;  mrs_2 = 1440 * 8; mrs_3 = 1440 * 11;  mrs_4 = 1440 * 24;  mrs_5 = 1440 * 29
+Intercranial haemhorrhage: mrs_0 = 1440 * 5; mrs_1 = 1440 * 4;  mrs_2 = 1440 * 5; mrs_3 = 1440 * 17;  mrs_4 = 1440 * 36;  mrs_5 = 1440 * 36
+non_stroke = 4320
+tia = 1440
+Where patients undergo thrombolysis, the sampled duration is modified by the following parameter: thrombolysis_los_save = 0.75
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="8"/>
+        <color theme="1"/>
+        <rFont val="Aptos"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">Opening/operating hours of resources
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color theme="1"/>
+        <rFont val="Aptos"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">Various parameters are used to determine what percentage of time the SDEC and advanced CT scanning capabilities are available and from what time of day they are available, defaulting to no availability for either. 
+These can be set independently of each other. 
+The model is primarily built to support one single uninterruped period of availability per day. 
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="8"/>
+        <color theme="1"/>
+        <rFont val="Aptos"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">Costs
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color theme="1"/>
+        <rFont val="Aptos"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">The cost of staffing the SDEC per minute is tracked with sdec_dr_cost_min = 0.50
+Per day overnight hyper-acute stroke unit bed costs are set as follows: inpatient_bed_cost = £876 and inpatient_bed_cost (thrombolysed patients) = £528.17 
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="8"/>
+        <color theme="1"/>
+        <rFont val="Aptos"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">
+Other</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color theme="1"/>
+        <rFont val="Aptos"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">
+The average Modified Rankin Scale score is determined with the parameter: mean_mrs = 2
+Patients are allocated a diagnosis value using a uniform distribution randing from 0 to 100. They are then categoriesed using the following boundaries: &lt;= 10 = intercranial haemhorrhage (ich); &lt;= 60 = ischaemic stroke (i); &lt;= 70 = tia; &lt;= 80 = stroke mimic; &gt; 80 = non-stroke</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">Seeds are generated using Numpy's seed sequence, which is itself primed by a user-provided seed (default 42) plus the run number. 
+Generators for each random number stream (one per activity) are set up independently using the sampling classes of the sim_tools package (v1.0.0), which each provided with a seed from the seed sequence. </t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">A single class of patient is used within the model, referenced as 'Patient' within the Python model code.
+These entities are the stroke and non-stroke patients who are seen within the pathway. 
+Key attributes are as follows:
+ID = a persistent identifier used to track a single patient through their full system journey
+onset_type = Categorisation of onset information: 0 : Known onset; 1 : Unknown onset but within CTP window; 2 : Unknown onset and outside CTP window
+mrs_type =  Modified Rankin Scale score at presentation (0–5). Drawn from an exponential distribution and capped at 5.  0 indicates no disability, while 5 represents severe disability. 
+mrs_discharge = Modified Rankin Scale score at discharge. Unlike mrs_type, which is set on patient generation, the mrs_discharge is set later by the model and may differ depending on the availability of different pathways within the model - e.g. a patient may have a lower MRS on discharge if the CT perfusion scanner availability permits them to have thrombolysis. 
+diagnosis = Raw randomised diagnostic value (0–100). 
+patient_diagnosis = Encoded diagnosis category: 0 : Intracerebral haemorrhage (ICH); 1 : Ischaemic stroke (I); 2 : Transient ischaemic attack (TIA); 3 : Stroke mimic; 4 : Non-stroke. This is mapped from the diagnosis patient attribute, using thresholds defined in the global parameter class `g`. 
+non_admission = a numerical score used to determine whether patients with a transient ischaemic attack (TIA) or stroke mimic symptoms are admitted. 
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Aptos"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">Tracking attributes
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Aptos"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">Various attributes are set as events occur in the model, allowing for post-hoc analysis of logs. 
+advanced_ct_pathway: Whether the patient enters an advanced CT imaging pathway (elsewhere referred to as CT perfusion scanning).
+sdec_pathway: Whether the patient is routed through the Same Day Emergency Care (SDEC) pathway.
+thrombolysis: Whether the patient receives thrombolysis.
+admission_avoidance: Whether the patient avoids an admission by being seen in SDEC instead.
+q_time_nurse, q_time_ward: Time spent waiting for nursing assessment/consultation, and time spent waiting for an inpatient ward bed respectively.
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Aptos"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">Unused attributes
+</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Aptos"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">Several attributes are created but not currently used by the published version of the model. They may be used in future versions of the model. </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Aptos"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">
+priority = a numerical triage priority level used for queue ordering. 
+thrombectomy = whether the patient receives mechanical thrombectomy
+</t>
+    </r>
+  </si>
+  <si>
+    <t>Details</t>
   </si>
 </sst>
 </file>
@@ -1118,14 +1178,14 @@
       <family val="2"/>
     </font>
     <font>
-      <sz val="9"/>
+      <sz val="8"/>
       <color theme="1"/>
       <name val="Aptos"/>
       <family val="2"/>
     </font>
     <font>
       <b/>
-      <sz val="9"/>
+      <sz val="8"/>
       <color theme="1"/>
       <name val="Aptos"/>
       <family val="2"/>
@@ -1303,7 +1363,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="46">
+  <cellXfs count="44">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -1338,33 +1398,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -1383,19 +1416,10 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1410,35 +1434,65 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1776,8 +1830,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B614ACE2-F615-4B99-BA80-52B48930DD2E}">
   <dimension ref="A1:E41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
-      <selection activeCell="D19" sqref="D19:D20"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1802,445 +1856,447 @@
     <row r="3" spans="1:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="2"/>
     </row>
-    <row r="4" spans="1:5" ht="63.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
         <v>2</v>
       </c>
       <c r="B4" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="C4" s="12" t="s">
+      <c r="C4" s="41" t="s">
         <v>4</v>
       </c>
-      <c r="D4" s="13"/>
+      <c r="D4" s="42"/>
       <c r="E4" s="5" t="s">
-        <v>5</v>
+        <v>80</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="B5" s="7"/>
+      <c r="C5" s="30"/>
+      <c r="D5" s="30"/>
+      <c r="E5" s="9"/>
+    </row>
+    <row r="6" spans="1:5" ht="252.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="B5" s="7"/>
-      <c r="C5" s="15"/>
-      <c r="D5" s="15"/>
-      <c r="E5" s="9"/>
-    </row>
-    <row r="6" spans="1:5" ht="268.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="21" t="s">
+      <c r="B6" s="18">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="C6" s="31" t="s">
         <v>7</v>
       </c>
-      <c r="B6" s="28">
-        <v>1.1000000000000001</v>
-      </c>
-      <c r="C6" s="17" t="s">
+      <c r="D6" s="31"/>
+      <c r="E6" s="8" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="363.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="20" t="s">
         <v>8</v>
       </c>
-      <c r="D6" s="17"/>
-      <c r="E6" s="8" t="s">
+      <c r="B7" s="8">
+        <v>1.2</v>
+      </c>
+      <c r="C7" s="43" t="s">
+        <v>9</v>
+      </c>
+      <c r="D7" s="43"/>
+      <c r="E7" s="21" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" ht="366.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="19" t="s">
+        <v>10</v>
+      </c>
+      <c r="B8" s="20">
+        <v>1.3</v>
+      </c>
+      <c r="C8" s="38" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="7" spans="1:5" ht="363.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="30" t="s">
-        <v>9</v>
-      </c>
-      <c r="B7" s="27">
-        <v>1.2</v>
-      </c>
-      <c r="C7" s="32" t="s">
-        <v>10</v>
-      </c>
-      <c r="D7" s="32"/>
-      <c r="E7" s="33" t="s">
+      <c r="D8" s="38"/>
+      <c r="E8" s="22" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="23" t="s">
+        <v>11</v>
+      </c>
+      <c r="B9" s="16"/>
+      <c r="C9" s="40"/>
+      <c r="D9" s="40"/>
+      <c r="E9" s="17"/>
+    </row>
+    <row r="10" spans="1:5" ht="143.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="12" t="s">
+        <v>12</v>
+      </c>
+      <c r="B10" s="12">
+        <v>2.1</v>
+      </c>
+      <c r="C10" s="31" t="s">
+        <v>13</v>
+      </c>
+      <c r="D10" s="31"/>
+      <c r="E10" s="12" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" ht="239.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="B11" s="13">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="C11" s="32" t="s">
+        <v>15</v>
+      </c>
+      <c r="D11" s="32"/>
+      <c r="E11" s="14" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="8" spans="1:5" ht="366.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="29" t="s">
-        <v>11</v>
-      </c>
-      <c r="B8" s="30">
-        <v>1.3</v>
-      </c>
-      <c r="C8" s="31" t="s">
-        <v>52</v>
-      </c>
-      <c r="D8" s="31"/>
-      <c r="E8" s="34" t="s">
+    <row r="12" spans="1:5" ht="168" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="B12" s="13">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="C12" s="32" t="s">
+        <v>17</v>
+      </c>
+      <c r="D12" s="32"/>
+      <c r="E12" s="14" t="s">
         <v>66</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="35" t="s">
-        <v>12</v>
-      </c>
-      <c r="B9" s="36"/>
-      <c r="C9" s="25"/>
-      <c r="D9" s="25"/>
-      <c r="E9" s="26"/>
-    </row>
-    <row r="10" spans="1:5" ht="143.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="21" t="s">
-        <v>13</v>
-      </c>
-      <c r="B10" s="21">
-        <v>2.1</v>
-      </c>
-      <c r="C10" s="17" t="s">
-        <v>14</v>
-      </c>
-      <c r="D10" s="17"/>
-      <c r="E10" s="21" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" ht="239.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="22" t="s">
-        <v>15</v>
-      </c>
-      <c r="B11" s="22">
-        <v>2.2000000000000002</v>
-      </c>
-      <c r="C11" s="19" t="s">
-        <v>16</v>
-      </c>
-      <c r="D11" s="19"/>
-      <c r="E11" s="23" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" ht="168" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="22" t="s">
-        <v>17</v>
-      </c>
-      <c r="B12" s="22">
-        <v>2.2999999999999998</v>
-      </c>
-      <c r="C12" s="19" t="s">
-        <v>18</v>
-      </c>
-      <c r="D12" s="19"/>
-      <c r="E12" s="23" t="s">
-        <v>68</v>
       </c>
     </row>
     <row r="13" spans="1:5" ht="158.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="10" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B13" s="10">
         <v>2.4</v>
       </c>
-      <c r="C13" s="20" t="s">
+      <c r="C13" s="29" t="s">
+        <v>19</v>
+      </c>
+      <c r="D13" s="29"/>
+      <c r="E13" s="11"/>
+    </row>
+    <row r="14" spans="1:5" ht="300.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="32" t="s">
         <v>20</v>
       </c>
-      <c r="D13" s="20"/>
-      <c r="E13" s="11"/>
-    </row>
-    <row r="14" spans="1:5" ht="300.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="19" t="s">
+      <c r="B14" s="32">
+        <v>2.5</v>
+      </c>
+      <c r="C14" s="32" t="s">
         <v>21</v>
       </c>
-      <c r="B14" s="19">
-        <v>2.5</v>
-      </c>
-      <c r="C14" s="19" t="s">
+      <c r="D14" s="32" t="s">
         <v>22</v>
       </c>
-      <c r="D14" s="19" t="s">
+      <c r="E14" s="36" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15" s="38"/>
+      <c r="B15" s="38"/>
+      <c r="C15" s="38"/>
+      <c r="D15" s="38"/>
+      <c r="E15" s="39"/>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A16" s="38"/>
+      <c r="B16" s="38"/>
+      <c r="C16" s="38"/>
+      <c r="D16" s="38"/>
+      <c r="E16" s="39"/>
+    </row>
+    <row r="17" spans="1:5" ht="234.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="38"/>
+      <c r="B17" s="38"/>
+      <c r="C17" s="35"/>
+      <c r="D17" s="35"/>
+      <c r="E17" s="37"/>
+    </row>
+    <row r="18" spans="1:5" ht="187.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="38"/>
+      <c r="B18" s="38"/>
+      <c r="C18" s="13" t="s">
         <v>23</v>
       </c>
-      <c r="E14" s="38" t="s">
+      <c r="D18" s="13" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A15" s="16"/>
-      <c r="B15" s="16"/>
-      <c r="C15" s="16"/>
-      <c r="D15" s="16"/>
-      <c r="E15" s="39"/>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A16" s="16"/>
-      <c r="B16" s="16"/>
-      <c r="C16" s="16"/>
-      <c r="D16" s="16"/>
-      <c r="E16" s="39"/>
-    </row>
-    <row r="17" spans="1:5" ht="234.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="16"/>
-      <c r="B17" s="16"/>
-      <c r="C17" s="18"/>
-      <c r="D17" s="18"/>
-      <c r="E17" s="40"/>
-    </row>
-    <row r="18" spans="1:5" ht="187.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="16"/>
-      <c r="B18" s="16"/>
-      <c r="C18" s="22" t="s">
+      <c r="E18" s="25" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" ht="204.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="38"/>
+      <c r="B19" s="38"/>
+      <c r="C19" s="32" t="s">
         <v>24</v>
       </c>
-      <c r="D18" s="22" t="s">
-        <v>62</v>
-      </c>
-      <c r="E18" s="41" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" ht="204.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="16"/>
-      <c r="B19" s="16"/>
-      <c r="C19" s="19" t="s">
+      <c r="D19" s="32" t="s">
         <v>25</v>
       </c>
-      <c r="D19" s="19" t="s">
+      <c r="E19" s="36" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" ht="157.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="38"/>
+      <c r="B20" s="38"/>
+      <c r="C20" s="35"/>
+      <c r="D20" s="35"/>
+      <c r="E20" s="37"/>
+    </row>
+    <row r="21" spans="1:5" ht="280.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="38"/>
+      <c r="B21" s="38"/>
+      <c r="C21" s="13" t="s">
         <v>26</v>
       </c>
-      <c r="E19" s="38" t="s">
+      <c r="D21" s="13" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="20" spans="1:5" ht="157.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="16"/>
-      <c r="B20" s="16"/>
-      <c r="C20" s="18"/>
-      <c r="D20" s="18"/>
-      <c r="E20" s="40"/>
-    </row>
-    <row r="21" spans="1:5" ht="280.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="16"/>
-      <c r="B21" s="16"/>
-      <c r="C21" s="22" t="s">
+      <c r="E21" s="14" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" ht="296.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A22" s="38"/>
+      <c r="B22" s="38"/>
+      <c r="C22" s="18" t="s">
         <v>27</v>
       </c>
-      <c r="D21" s="22" t="s">
-        <v>63</v>
-      </c>
-      <c r="E21" s="23" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" ht="296.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="16"/>
-      <c r="B22" s="16"/>
-      <c r="C22" s="28" t="s">
+      <c r="D22" s="18" t="s">
         <v>28</v>
       </c>
-      <c r="D22" s="28" t="s">
-        <v>29</v>
-      </c>
-      <c r="E22" s="45" t="s">
-        <v>69</v>
+      <c r="E22" s="27" t="s">
+        <v>67</v>
       </c>
     </row>
     <row r="23" spans="1:5" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="B23" s="7"/>
+      <c r="C23" s="33"/>
+      <c r="D23" s="33"/>
+      <c r="E23" s="9"/>
+    </row>
+    <row r="24" spans="1:5" ht="229.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A24" s="12" t="s">
         <v>30</v>
       </c>
-      <c r="B23" s="7"/>
-      <c r="C23" s="14"/>
-      <c r="D23" s="14"/>
-      <c r="E23" s="9"/>
-    </row>
-    <row r="24" spans="1:5" ht="229.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="21" t="s">
+      <c r="B24" s="12">
+        <v>3.1</v>
+      </c>
+      <c r="C24" s="31" t="s">
+        <v>52</v>
+      </c>
+      <c r="D24" s="31"/>
+      <c r="E24" s="24"/>
+    </row>
+    <row r="25" spans="1:5" ht="173.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A25" s="13" t="s">
         <v>31</v>
       </c>
-      <c r="B24" s="21">
-        <v>3.1</v>
-      </c>
-      <c r="C24" s="17" t="s">
+      <c r="B25" s="13">
+        <v>3.2</v>
+      </c>
+      <c r="C25" s="32" t="s">
+        <v>32</v>
+      </c>
+      <c r="D25" s="32"/>
+      <c r="E25" s="14"/>
+    </row>
+    <row r="26" spans="1:5" ht="409.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A26" s="13" t="s">
+        <v>33</v>
+      </c>
+      <c r="B26" s="13">
+        <v>3.3</v>
+      </c>
+      <c r="C26" s="32" t="s">
         <v>53</v>
       </c>
-      <c r="D24" s="17"/>
-      <c r="E24" s="37"/>
-    </row>
-    <row r="25" spans="1:5" ht="173.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="22" t="s">
-        <v>32</v>
-      </c>
-      <c r="B25" s="22">
-        <v>3.2</v>
-      </c>
-      <c r="C25" s="19" t="s">
-        <v>33</v>
-      </c>
-      <c r="D25" s="19"/>
-      <c r="E25" s="23"/>
-    </row>
-    <row r="26" spans="1:5" ht="409.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="22" t="s">
+      <c r="D26" s="32"/>
+      <c r="E26" s="28" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" ht="174" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A27" s="15" t="s">
         <v>34</v>
       </c>
-      <c r="B26" s="22">
-        <v>3.3</v>
-      </c>
-      <c r="C26" s="19" t="s">
-        <v>54</v>
-      </c>
-      <c r="D26" s="19"/>
-      <c r="E26" s="42" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5" ht="174" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="24" t="s">
+      <c r="B27" s="15">
+        <v>3.4</v>
+      </c>
+      <c r="C27" s="34" t="s">
         <v>35</v>
       </c>
-      <c r="B27" s="24">
-        <v>3.4</v>
-      </c>
-      <c r="C27" s="44" t="s">
-        <v>36</v>
-      </c>
-      <c r="D27" s="44"/>
-      <c r="E27" s="43"/>
+      <c r="D27" s="34"/>
+      <c r="E27" s="26"/>
     </row>
     <row r="28" spans="1:5" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A28" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="B28" s="7"/>
+      <c r="C28" s="33"/>
+      <c r="D28" s="33"/>
+      <c r="E28" s="9"/>
+    </row>
+    <row r="29" spans="1:5" ht="220.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A29" s="12" t="s">
         <v>37</v>
       </c>
-      <c r="B28" s="7"/>
-      <c r="C28" s="14"/>
-      <c r="D28" s="14"/>
-      <c r="E28" s="9"/>
-    </row>
-    <row r="29" spans="1:5" ht="220.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="21" t="s">
+      <c r="B29" s="12">
+        <v>4.0999999999999996</v>
+      </c>
+      <c r="C29" s="31" t="s">
+        <v>54</v>
+      </c>
+      <c r="D29" s="31"/>
+      <c r="E29" s="24" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" ht="63" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A30" s="13" t="s">
         <v>38</v>
       </c>
-      <c r="B29" s="21">
-        <v>4.0999999999999996</v>
-      </c>
-      <c r="C29" s="17" t="s">
-        <v>55</v>
-      </c>
-      <c r="D29" s="17"/>
-      <c r="E29" s="37" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="30" spans="1:5" ht="63" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="22" t="s">
+      <c r="B30" s="13">
+        <v>4.2</v>
+      </c>
+      <c r="C30" s="32" t="s">
         <v>39</v>
       </c>
-      <c r="B30" s="22">
-        <v>4.2</v>
-      </c>
-      <c r="C30" s="19" t="s">
-        <v>40</v>
-      </c>
-      <c r="D30" s="19"/>
-      <c r="E30" s="23" t="s">
-        <v>76</v>
+      <c r="D30" s="32"/>
+      <c r="E30" s="14" t="s">
+        <v>74</v>
       </c>
     </row>
     <row r="31" spans="1:5" ht="215.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A31" s="8" t="s">
-        <v>41</v>
-      </c>
-      <c r="B31" s="24">
+        <v>40</v>
+      </c>
+      <c r="B31" s="15">
         <v>4.3</v>
       </c>
-      <c r="C31" s="44" t="s">
-        <v>64</v>
-      </c>
-      <c r="D31" s="44"/>
-      <c r="E31" s="43" t="s">
-        <v>74</v>
+      <c r="C31" s="34" t="s">
+        <v>62</v>
+      </c>
+      <c r="D31" s="34"/>
+      <c r="E31" s="26" t="s">
+        <v>72</v>
       </c>
     </row>
     <row r="32" spans="1:5" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A32" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="B32" s="7"/>
+      <c r="C32" s="33"/>
+      <c r="D32" s="33"/>
+      <c r="E32" s="9"/>
+    </row>
+    <row r="33" spans="1:5" ht="347.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A33" s="12" t="s">
         <v>42</v>
       </c>
-      <c r="B32" s="7"/>
-      <c r="C32" s="14"/>
-      <c r="D32" s="14"/>
-      <c r="E32" s="9"/>
-    </row>
-    <row r="33" spans="1:5" ht="347.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A33" s="21" t="s">
+      <c r="B33" s="12">
+        <v>5.0999999999999996</v>
+      </c>
+      <c r="C33" s="31" t="s">
+        <v>55</v>
+      </c>
+      <c r="D33" s="31"/>
+      <c r="E33" s="24" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" ht="141.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A34" s="13" t="s">
         <v>43</v>
       </c>
-      <c r="B33" s="21">
-        <v>5.0999999999999996</v>
-      </c>
-      <c r="C33" s="17" t="s">
+      <c r="B34" s="13">
+        <v>5.2</v>
+      </c>
+      <c r="C34" s="32" t="s">
         <v>56</v>
       </c>
-      <c r="D33" s="17"/>
-      <c r="E33" s="37" t="s">
+      <c r="D34" s="32"/>
+      <c r="E34" s="14" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" ht="306" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A35" s="13" t="s">
+        <v>44</v>
+      </c>
+      <c r="B35" s="13">
+        <v>5.3</v>
+      </c>
+      <c r="C35" s="32" t="s">
+        <v>57</v>
+      </c>
+      <c r="D35" s="32"/>
+      <c r="E35" s="14" t="s">
         <v>71</v>
-      </c>
-    </row>
-    <row r="34" spans="1:5" ht="141.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A34" s="22" t="s">
-        <v>44</v>
-      </c>
-      <c r="B34" s="22">
-        <v>5.2</v>
-      </c>
-      <c r="C34" s="19" t="s">
-        <v>57</v>
-      </c>
-      <c r="D34" s="19"/>
-      <c r="E34" s="23"/>
-    </row>
-    <row r="35" spans="1:5" ht="306" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A35" s="22" t="s">
-        <v>45</v>
-      </c>
-      <c r="B35" s="22">
-        <v>5.3</v>
-      </c>
-      <c r="C35" s="19" t="s">
-        <v>58</v>
-      </c>
-      <c r="D35" s="19"/>
-      <c r="E35" s="23" t="s">
-        <v>73</v>
       </c>
     </row>
     <row r="36" spans="1:5" ht="117" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A36" s="10" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B36" s="10">
         <v>5.4</v>
       </c>
-      <c r="C36" s="20" t="s">
-        <v>47</v>
-      </c>
-      <c r="D36" s="20"/>
+      <c r="C36" s="29" t="s">
+        <v>46</v>
+      </c>
+      <c r="D36" s="29"/>
       <c r="E36" s="11" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
     </row>
     <row r="37" spans="1:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A37" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="B37" s="7"/>
+      <c r="C37" s="30"/>
+      <c r="D37" s="30"/>
+      <c r="E37" s="9"/>
+    </row>
+    <row r="38" spans="1:5" ht="139.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A38" s="12" t="s">
         <v>48</v>
       </c>
-      <c r="B37" s="7"/>
-      <c r="C37" s="15"/>
-      <c r="D37" s="15"/>
-      <c r="E37" s="9"/>
-    </row>
-    <row r="38" spans="1:5" ht="139.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="21" t="s">
+      <c r="B38" s="12">
+        <v>6.1</v>
+      </c>
+      <c r="C38" s="31" t="s">
         <v>49</v>
       </c>
-      <c r="B38" s="21">
-        <v>6.1</v>
-      </c>
-      <c r="C38" s="17" t="s">
-        <v>50</v>
-      </c>
-      <c r="D38" s="17"/>
-      <c r="E38" s="37" t="s">
-        <v>70</v>
+      <c r="D38" s="31"/>
+      <c r="E38" s="24" t="s">
+        <v>68</v>
       </c>
     </row>
     <row r="39" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
@@ -2251,22 +2307,15 @@
     </row>
   </sheetData>
   <mergeCells count="34">
-    <mergeCell ref="C36:D36"/>
-    <mergeCell ref="C37:D37"/>
-    <mergeCell ref="C38:D38"/>
-    <mergeCell ref="C35:D35"/>
-    <mergeCell ref="C34:D34"/>
-    <mergeCell ref="C32:D32"/>
-    <mergeCell ref="C33:D33"/>
-    <mergeCell ref="C30:D30"/>
-    <mergeCell ref="C31:D31"/>
-    <mergeCell ref="C28:D28"/>
-    <mergeCell ref="C29:D29"/>
-    <mergeCell ref="C27:D27"/>
-    <mergeCell ref="C26:D26"/>
-    <mergeCell ref="C25:D25"/>
-    <mergeCell ref="C23:D23"/>
-    <mergeCell ref="C24:D24"/>
+    <mergeCell ref="C4:D4"/>
+    <mergeCell ref="C5:D5"/>
+    <mergeCell ref="C6:D6"/>
+    <mergeCell ref="C7:D7"/>
+    <mergeCell ref="C11:D11"/>
+    <mergeCell ref="C12:D12"/>
+    <mergeCell ref="C9:D9"/>
+    <mergeCell ref="C10:D10"/>
+    <mergeCell ref="C8:D8"/>
     <mergeCell ref="D19:D20"/>
     <mergeCell ref="E19:E20"/>
     <mergeCell ref="C13:D13"/>
@@ -2276,15 +2325,22 @@
     <mergeCell ref="D14:D17"/>
     <mergeCell ref="E14:E17"/>
     <mergeCell ref="C19:C20"/>
-    <mergeCell ref="C11:D11"/>
-    <mergeCell ref="C12:D12"/>
-    <mergeCell ref="C9:D9"/>
-    <mergeCell ref="C10:D10"/>
-    <mergeCell ref="C8:D8"/>
-    <mergeCell ref="C4:D4"/>
-    <mergeCell ref="C5:D5"/>
-    <mergeCell ref="C6:D6"/>
-    <mergeCell ref="C7:D7"/>
+    <mergeCell ref="C27:D27"/>
+    <mergeCell ref="C26:D26"/>
+    <mergeCell ref="C25:D25"/>
+    <mergeCell ref="C23:D23"/>
+    <mergeCell ref="C24:D24"/>
+    <mergeCell ref="C32:D32"/>
+    <mergeCell ref="C33:D33"/>
+    <mergeCell ref="C30:D30"/>
+    <mergeCell ref="C31:D31"/>
+    <mergeCell ref="C28:D28"/>
+    <mergeCell ref="C29:D29"/>
+    <mergeCell ref="C36:D36"/>
+    <mergeCell ref="C37:D37"/>
+    <mergeCell ref="C38:D38"/>
+    <mergeCell ref="C35:D35"/>
+    <mergeCell ref="C34:D34"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId1"/>

</xml_diff>